<commit_message>
eerste test dashboard en extra methode (studentsinGroup) in groupDAO
</commit_message>
<xml_diff>
--- a/Specificaties en eisen/Scene Overview.xlsx
+++ b/Specificaties en eisen/Scene Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Make IT Work\Quizmaster\Quizmaster\Specificaties en eisen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BCB0F8-B3E2-4FF9-B595-0326F3781FA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5986F60-836A-47CE-8B5C-2A54D9B546FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
   <si>
     <t>Table 1</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>CoordinatorDashboardController</t>
+  </si>
+  <si>
+    <t>NewQuiz, New Question</t>
   </si>
 </sst>
 </file>
@@ -602,9 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -613,6 +613,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1812,7 +1815,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1829,17 +1832,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:256" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1871,31 +1874,31 @@
       </c>
     </row>
     <row r="3" spans="1:256" s="12" customFormat="1" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="11"/>
@@ -4587,8 +4590,12 @@
         <v>62</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>

</xml_diff>

<commit_message>
Cascading delete van course/group mogelijk met behoud van user
</commit_message>
<xml_diff>
--- a/Specificaties en eisen/Scene Overview.xlsx
+++ b/Specificaties en eisen/Scene Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Make IT Work\Quizmaster\Quizmaster\Specificaties en eisen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5986F60-836A-47CE-8B5C-2A54D9B546FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE94DF07-A425-44C9-8F9D-AD154D3A0E68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,12 +418,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,7 +541,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -585,24 +579,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1812,10 +1788,10 @@
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1832,17 +1808,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:256" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1874,31 +1850,31 @@
       </c>
     </row>
     <row r="3" spans="1:256" s="12" customFormat="1" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="11"/>
@@ -2149,34 +2125,281 @@
       <c r="IU3" s="11"/>
       <c r="IV3" s="11"/>
     </row>
-    <row r="4" spans="1:256" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:256" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="11"/>
+      <c r="AS4" s="11"/>
+      <c r="AT4" s="11"/>
+      <c r="AU4" s="11"/>
+      <c r="AV4" s="11"/>
+      <c r="AW4" s="11"/>
+      <c r="AX4" s="11"/>
+      <c r="AY4" s="11"/>
+      <c r="AZ4" s="11"/>
+      <c r="BA4" s="11"/>
+      <c r="BB4" s="11"/>
+      <c r="BC4" s="11"/>
+      <c r="BD4" s="11"/>
+      <c r="BE4" s="11"/>
+      <c r="BF4" s="11"/>
+      <c r="BG4" s="11"/>
+      <c r="BH4" s="11"/>
+      <c r="BI4" s="11"/>
+      <c r="BJ4" s="11"/>
+      <c r="BK4" s="11"/>
+      <c r="BL4" s="11"/>
+      <c r="BM4" s="11"/>
+      <c r="BN4" s="11"/>
+      <c r="BO4" s="11"/>
+      <c r="BP4" s="11"/>
+      <c r="BQ4" s="11"/>
+      <c r="BR4" s="11"/>
+      <c r="BS4" s="11"/>
+      <c r="BT4" s="11"/>
+      <c r="BU4" s="11"/>
+      <c r="BV4" s="11"/>
+      <c r="BW4" s="11"/>
+      <c r="BX4" s="11"/>
+      <c r="BY4" s="11"/>
+      <c r="BZ4" s="11"/>
+      <c r="CA4" s="11"/>
+      <c r="CB4" s="11"/>
+      <c r="CC4" s="11"/>
+      <c r="CD4" s="11"/>
+      <c r="CE4" s="11"/>
+      <c r="CF4" s="11"/>
+      <c r="CG4" s="11"/>
+      <c r="CH4" s="11"/>
+      <c r="CI4" s="11"/>
+      <c r="CJ4" s="11"/>
+      <c r="CK4" s="11"/>
+      <c r="CL4" s="11"/>
+      <c r="CM4" s="11"/>
+      <c r="CN4" s="11"/>
+      <c r="CO4" s="11"/>
+      <c r="CP4" s="11"/>
+      <c r="CQ4" s="11"/>
+      <c r="CR4" s="11"/>
+      <c r="CS4" s="11"/>
+      <c r="CT4" s="11"/>
+      <c r="CU4" s="11"/>
+      <c r="CV4" s="11"/>
+      <c r="CW4" s="11"/>
+      <c r="CX4" s="11"/>
+      <c r="CY4" s="11"/>
+      <c r="CZ4" s="11"/>
+      <c r="DA4" s="11"/>
+      <c r="DB4" s="11"/>
+      <c r="DC4" s="11"/>
+      <c r="DD4" s="11"/>
+      <c r="DE4" s="11"/>
+      <c r="DF4" s="11"/>
+      <c r="DG4" s="11"/>
+      <c r="DH4" s="11"/>
+      <c r="DI4" s="11"/>
+      <c r="DJ4" s="11"/>
+      <c r="DK4" s="11"/>
+      <c r="DL4" s="11"/>
+      <c r="DM4" s="11"/>
+      <c r="DN4" s="11"/>
+      <c r="DO4" s="11"/>
+      <c r="DP4" s="11"/>
+      <c r="DQ4" s="11"/>
+      <c r="DR4" s="11"/>
+      <c r="DS4" s="11"/>
+      <c r="DT4" s="11"/>
+      <c r="DU4" s="11"/>
+      <c r="DV4" s="11"/>
+      <c r="DW4" s="11"/>
+      <c r="DX4" s="11"/>
+      <c r="DY4" s="11"/>
+      <c r="DZ4" s="11"/>
+      <c r="EA4" s="11"/>
+      <c r="EB4" s="11"/>
+      <c r="EC4" s="11"/>
+      <c r="ED4" s="11"/>
+      <c r="EE4" s="11"/>
+      <c r="EF4" s="11"/>
+      <c r="EG4" s="11"/>
+      <c r="EH4" s="11"/>
+      <c r="EI4" s="11"/>
+      <c r="EJ4" s="11"/>
+      <c r="EK4" s="11"/>
+      <c r="EL4" s="11"/>
+      <c r="EM4" s="11"/>
+      <c r="EN4" s="11"/>
+      <c r="EO4" s="11"/>
+      <c r="EP4" s="11"/>
+      <c r="EQ4" s="11"/>
+      <c r="ER4" s="11"/>
+      <c r="ES4" s="11"/>
+      <c r="ET4" s="11"/>
+      <c r="EU4" s="11"/>
+      <c r="EV4" s="11"/>
+      <c r="EW4" s="11"/>
+      <c r="EX4" s="11"/>
+      <c r="EY4" s="11"/>
+      <c r="EZ4" s="11"/>
+      <c r="FA4" s="11"/>
+      <c r="FB4" s="11"/>
+      <c r="FC4" s="11"/>
+      <c r="FD4" s="11"/>
+      <c r="FE4" s="11"/>
+      <c r="FF4" s="11"/>
+      <c r="FG4" s="11"/>
+      <c r="FH4" s="11"/>
+      <c r="FI4" s="11"/>
+      <c r="FJ4" s="11"/>
+      <c r="FK4" s="11"/>
+      <c r="FL4" s="11"/>
+      <c r="FM4" s="11"/>
+      <c r="FN4" s="11"/>
+      <c r="FO4" s="11"/>
+      <c r="FP4" s="11"/>
+      <c r="FQ4" s="11"/>
+      <c r="FR4" s="11"/>
+      <c r="FS4" s="11"/>
+      <c r="FT4" s="11"/>
+      <c r="FU4" s="11"/>
+      <c r="FV4" s="11"/>
+      <c r="FW4" s="11"/>
+      <c r="FX4" s="11"/>
+      <c r="FY4" s="11"/>
+      <c r="FZ4" s="11"/>
+      <c r="GA4" s="11"/>
+      <c r="GB4" s="11"/>
+      <c r="GC4" s="11"/>
+      <c r="GD4" s="11"/>
+      <c r="GE4" s="11"/>
+      <c r="GF4" s="11"/>
+      <c r="GG4" s="11"/>
+      <c r="GH4" s="11"/>
+      <c r="GI4" s="11"/>
+      <c r="GJ4" s="11"/>
+      <c r="GK4" s="11"/>
+      <c r="GL4" s="11"/>
+      <c r="GM4" s="11"/>
+      <c r="GN4" s="11"/>
+      <c r="GO4" s="11"/>
+      <c r="GP4" s="11"/>
+      <c r="GQ4" s="11"/>
+      <c r="GR4" s="11"/>
+      <c r="GS4" s="11"/>
+      <c r="GT4" s="11"/>
+      <c r="GU4" s="11"/>
+      <c r="GV4" s="11"/>
+      <c r="GW4" s="11"/>
+      <c r="GX4" s="11"/>
+      <c r="GY4" s="11"/>
+      <c r="GZ4" s="11"/>
+      <c r="HA4" s="11"/>
+      <c r="HB4" s="11"/>
+      <c r="HC4" s="11"/>
+      <c r="HD4" s="11"/>
+      <c r="HE4" s="11"/>
+      <c r="HF4" s="11"/>
+      <c r="HG4" s="11"/>
+      <c r="HH4" s="11"/>
+      <c r="HI4" s="11"/>
+      <c r="HJ4" s="11"/>
+      <c r="HK4" s="11"/>
+      <c r="HL4" s="11"/>
+      <c r="HM4" s="11"/>
+      <c r="HN4" s="11"/>
+      <c r="HO4" s="11"/>
+      <c r="HP4" s="11"/>
+      <c r="HQ4" s="11"/>
+      <c r="HR4" s="11"/>
+      <c r="HS4" s="11"/>
+      <c r="HT4" s="11"/>
+      <c r="HU4" s="11"/>
+      <c r="HV4" s="11"/>
+      <c r="HW4" s="11"/>
+      <c r="HX4" s="11"/>
+      <c r="HY4" s="11"/>
+      <c r="HZ4" s="11"/>
+      <c r="IA4" s="11"/>
+      <c r="IB4" s="11"/>
+      <c r="IC4" s="11"/>
+      <c r="ID4" s="11"/>
+      <c r="IE4" s="11"/>
+      <c r="IF4" s="11"/>
+      <c r="IG4" s="11"/>
+      <c r="IH4" s="11"/>
+      <c r="II4" s="11"/>
+      <c r="IJ4" s="11"/>
+      <c r="IK4" s="11"/>
+      <c r="IL4" s="11"/>
+      <c r="IM4" s="11"/>
+      <c r="IN4" s="11"/>
+      <c r="IO4" s="11"/>
+      <c r="IP4" s="11"/>
+      <c r="IQ4" s="11"/>
+      <c r="IR4" s="11"/>
+      <c r="IS4" s="11"/>
+      <c r="IT4" s="11"/>
+      <c r="IU4" s="11"/>
+      <c r="IV4" s="11"/>
     </row>
     <row r="5" spans="1:256" s="12" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -3324,32 +3547,279 @@
       <c r="IU10" s="11"/>
       <c r="IV10" s="11"/>
     </row>
-    <row r="11" spans="1:256" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:256" s="12" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
+      <c r="AQ11" s="11"/>
+      <c r="AR11" s="11"/>
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11"/>
+      <c r="AV11" s="11"/>
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="11"/>
+      <c r="AY11" s="11"/>
+      <c r="AZ11" s="11"/>
+      <c r="BA11" s="11"/>
+      <c r="BB11" s="11"/>
+      <c r="BC11" s="11"/>
+      <c r="BD11" s="11"/>
+      <c r="BE11" s="11"/>
+      <c r="BF11" s="11"/>
+      <c r="BG11" s="11"/>
+      <c r="BH11" s="11"/>
+      <c r="BI11" s="11"/>
+      <c r="BJ11" s="11"/>
+      <c r="BK11" s="11"/>
+      <c r="BL11" s="11"/>
+      <c r="BM11" s="11"/>
+      <c r="BN11" s="11"/>
+      <c r="BO11" s="11"/>
+      <c r="BP11" s="11"/>
+      <c r="BQ11" s="11"/>
+      <c r="BR11" s="11"/>
+      <c r="BS11" s="11"/>
+      <c r="BT11" s="11"/>
+      <c r="BU11" s="11"/>
+      <c r="BV11" s="11"/>
+      <c r="BW11" s="11"/>
+      <c r="BX11" s="11"/>
+      <c r="BY11" s="11"/>
+      <c r="BZ11" s="11"/>
+      <c r="CA11" s="11"/>
+      <c r="CB11" s="11"/>
+      <c r="CC11" s="11"/>
+      <c r="CD11" s="11"/>
+      <c r="CE11" s="11"/>
+      <c r="CF11" s="11"/>
+      <c r="CG11" s="11"/>
+      <c r="CH11" s="11"/>
+      <c r="CI11" s="11"/>
+      <c r="CJ11" s="11"/>
+      <c r="CK11" s="11"/>
+      <c r="CL11" s="11"/>
+      <c r="CM11" s="11"/>
+      <c r="CN11" s="11"/>
+      <c r="CO11" s="11"/>
+      <c r="CP11" s="11"/>
+      <c r="CQ11" s="11"/>
+      <c r="CR11" s="11"/>
+      <c r="CS11" s="11"/>
+      <c r="CT11" s="11"/>
+      <c r="CU11" s="11"/>
+      <c r="CV11" s="11"/>
+      <c r="CW11" s="11"/>
+      <c r="CX11" s="11"/>
+      <c r="CY11" s="11"/>
+      <c r="CZ11" s="11"/>
+      <c r="DA11" s="11"/>
+      <c r="DB11" s="11"/>
+      <c r="DC11" s="11"/>
+      <c r="DD11" s="11"/>
+      <c r="DE11" s="11"/>
+      <c r="DF11" s="11"/>
+      <c r="DG11" s="11"/>
+      <c r="DH11" s="11"/>
+      <c r="DI11" s="11"/>
+      <c r="DJ11" s="11"/>
+      <c r="DK11" s="11"/>
+      <c r="DL11" s="11"/>
+      <c r="DM11" s="11"/>
+      <c r="DN11" s="11"/>
+      <c r="DO11" s="11"/>
+      <c r="DP11" s="11"/>
+      <c r="DQ11" s="11"/>
+      <c r="DR11" s="11"/>
+      <c r="DS11" s="11"/>
+      <c r="DT11" s="11"/>
+      <c r="DU11" s="11"/>
+      <c r="DV11" s="11"/>
+      <c r="DW11" s="11"/>
+      <c r="DX11" s="11"/>
+      <c r="DY11" s="11"/>
+      <c r="DZ11" s="11"/>
+      <c r="EA11" s="11"/>
+      <c r="EB11" s="11"/>
+      <c r="EC11" s="11"/>
+      <c r="ED11" s="11"/>
+      <c r="EE11" s="11"/>
+      <c r="EF11" s="11"/>
+      <c r="EG11" s="11"/>
+      <c r="EH11" s="11"/>
+      <c r="EI11" s="11"/>
+      <c r="EJ11" s="11"/>
+      <c r="EK11" s="11"/>
+      <c r="EL11" s="11"/>
+      <c r="EM11" s="11"/>
+      <c r="EN11" s="11"/>
+      <c r="EO11" s="11"/>
+      <c r="EP11" s="11"/>
+      <c r="EQ11" s="11"/>
+      <c r="ER11" s="11"/>
+      <c r="ES11" s="11"/>
+      <c r="ET11" s="11"/>
+      <c r="EU11" s="11"/>
+      <c r="EV11" s="11"/>
+      <c r="EW11" s="11"/>
+      <c r="EX11" s="11"/>
+      <c r="EY11" s="11"/>
+      <c r="EZ11" s="11"/>
+      <c r="FA11" s="11"/>
+      <c r="FB11" s="11"/>
+      <c r="FC11" s="11"/>
+      <c r="FD11" s="11"/>
+      <c r="FE11" s="11"/>
+      <c r="FF11" s="11"/>
+      <c r="FG11" s="11"/>
+      <c r="FH11" s="11"/>
+      <c r="FI11" s="11"/>
+      <c r="FJ11" s="11"/>
+      <c r="FK11" s="11"/>
+      <c r="FL11" s="11"/>
+      <c r="FM11" s="11"/>
+      <c r="FN11" s="11"/>
+      <c r="FO11" s="11"/>
+      <c r="FP11" s="11"/>
+      <c r="FQ11" s="11"/>
+      <c r="FR11" s="11"/>
+      <c r="FS11" s="11"/>
+      <c r="FT11" s="11"/>
+      <c r="FU11" s="11"/>
+      <c r="FV11" s="11"/>
+      <c r="FW11" s="11"/>
+      <c r="FX11" s="11"/>
+      <c r="FY11" s="11"/>
+      <c r="FZ11" s="11"/>
+      <c r="GA11" s="11"/>
+      <c r="GB11" s="11"/>
+      <c r="GC11" s="11"/>
+      <c r="GD11" s="11"/>
+      <c r="GE11" s="11"/>
+      <c r="GF11" s="11"/>
+      <c r="GG11" s="11"/>
+      <c r="GH11" s="11"/>
+      <c r="GI11" s="11"/>
+      <c r="GJ11" s="11"/>
+      <c r="GK11" s="11"/>
+      <c r="GL11" s="11"/>
+      <c r="GM11" s="11"/>
+      <c r="GN11" s="11"/>
+      <c r="GO11" s="11"/>
+      <c r="GP11" s="11"/>
+      <c r="GQ11" s="11"/>
+      <c r="GR11" s="11"/>
+      <c r="GS11" s="11"/>
+      <c r="GT11" s="11"/>
+      <c r="GU11" s="11"/>
+      <c r="GV11" s="11"/>
+      <c r="GW11" s="11"/>
+      <c r="GX11" s="11"/>
+      <c r="GY11" s="11"/>
+      <c r="GZ11" s="11"/>
+      <c r="HA11" s="11"/>
+      <c r="HB11" s="11"/>
+      <c r="HC11" s="11"/>
+      <c r="HD11" s="11"/>
+      <c r="HE11" s="11"/>
+      <c r="HF11" s="11"/>
+      <c r="HG11" s="11"/>
+      <c r="HH11" s="11"/>
+      <c r="HI11" s="11"/>
+      <c r="HJ11" s="11"/>
+      <c r="HK11" s="11"/>
+      <c r="HL11" s="11"/>
+      <c r="HM11" s="11"/>
+      <c r="HN11" s="11"/>
+      <c r="HO11" s="11"/>
+      <c r="HP11" s="11"/>
+      <c r="HQ11" s="11"/>
+      <c r="HR11" s="11"/>
+      <c r="HS11" s="11"/>
+      <c r="HT11" s="11"/>
+      <c r="HU11" s="11"/>
+      <c r="HV11" s="11"/>
+      <c r="HW11" s="11"/>
+      <c r="HX11" s="11"/>
+      <c r="HY11" s="11"/>
+      <c r="HZ11" s="11"/>
+      <c r="IA11" s="11"/>
+      <c r="IB11" s="11"/>
+      <c r="IC11" s="11"/>
+      <c r="ID11" s="11"/>
+      <c r="IE11" s="11"/>
+      <c r="IF11" s="11"/>
+      <c r="IG11" s="11"/>
+      <c r="IH11" s="11"/>
+      <c r="II11" s="11"/>
+      <c r="IJ11" s="11"/>
+      <c r="IK11" s="11"/>
+      <c r="IL11" s="11"/>
+      <c r="IM11" s="11"/>
+      <c r="IN11" s="11"/>
+      <c r="IO11" s="11"/>
+      <c r="IP11" s="11"/>
+      <c r="IQ11" s="11"/>
+      <c r="IR11" s="11"/>
+      <c r="IS11" s="11"/>
+      <c r="IT11" s="11"/>
+      <c r="IU11" s="11"/>
+      <c r="IV11" s="11"/>
     </row>
     <row r="12" spans="1:256" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -3627,34 +4097,281 @@
       <c r="IU12" s="11"/>
       <c r="IV12" s="11"/>
     </row>
-    <row r="13" spans="1:256" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:256" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="11"/>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11"/>
+      <c r="AQ13" s="11"/>
+      <c r="AR13" s="11"/>
+      <c r="AS13" s="11"/>
+      <c r="AT13" s="11"/>
+      <c r="AU13" s="11"/>
+      <c r="AV13" s="11"/>
+      <c r="AW13" s="11"/>
+      <c r="AX13" s="11"/>
+      <c r="AY13" s="11"/>
+      <c r="AZ13" s="11"/>
+      <c r="BA13" s="11"/>
+      <c r="BB13" s="11"/>
+      <c r="BC13" s="11"/>
+      <c r="BD13" s="11"/>
+      <c r="BE13" s="11"/>
+      <c r="BF13" s="11"/>
+      <c r="BG13" s="11"/>
+      <c r="BH13" s="11"/>
+      <c r="BI13" s="11"/>
+      <c r="BJ13" s="11"/>
+      <c r="BK13" s="11"/>
+      <c r="BL13" s="11"/>
+      <c r="BM13" s="11"/>
+      <c r="BN13" s="11"/>
+      <c r="BO13" s="11"/>
+      <c r="BP13" s="11"/>
+      <c r="BQ13" s="11"/>
+      <c r="BR13" s="11"/>
+      <c r="BS13" s="11"/>
+      <c r="BT13" s="11"/>
+      <c r="BU13" s="11"/>
+      <c r="BV13" s="11"/>
+      <c r="BW13" s="11"/>
+      <c r="BX13" s="11"/>
+      <c r="BY13" s="11"/>
+      <c r="BZ13" s="11"/>
+      <c r="CA13" s="11"/>
+      <c r="CB13" s="11"/>
+      <c r="CC13" s="11"/>
+      <c r="CD13" s="11"/>
+      <c r="CE13" s="11"/>
+      <c r="CF13" s="11"/>
+      <c r="CG13" s="11"/>
+      <c r="CH13" s="11"/>
+      <c r="CI13" s="11"/>
+      <c r="CJ13" s="11"/>
+      <c r="CK13" s="11"/>
+      <c r="CL13" s="11"/>
+      <c r="CM13" s="11"/>
+      <c r="CN13" s="11"/>
+      <c r="CO13" s="11"/>
+      <c r="CP13" s="11"/>
+      <c r="CQ13" s="11"/>
+      <c r="CR13" s="11"/>
+      <c r="CS13" s="11"/>
+      <c r="CT13" s="11"/>
+      <c r="CU13" s="11"/>
+      <c r="CV13" s="11"/>
+      <c r="CW13" s="11"/>
+      <c r="CX13" s="11"/>
+      <c r="CY13" s="11"/>
+      <c r="CZ13" s="11"/>
+      <c r="DA13" s="11"/>
+      <c r="DB13" s="11"/>
+      <c r="DC13" s="11"/>
+      <c r="DD13" s="11"/>
+      <c r="DE13" s="11"/>
+      <c r="DF13" s="11"/>
+      <c r="DG13" s="11"/>
+      <c r="DH13" s="11"/>
+      <c r="DI13" s="11"/>
+      <c r="DJ13" s="11"/>
+      <c r="DK13" s="11"/>
+      <c r="DL13" s="11"/>
+      <c r="DM13" s="11"/>
+      <c r="DN13" s="11"/>
+      <c r="DO13" s="11"/>
+      <c r="DP13" s="11"/>
+      <c r="DQ13" s="11"/>
+      <c r="DR13" s="11"/>
+      <c r="DS13" s="11"/>
+      <c r="DT13" s="11"/>
+      <c r="DU13" s="11"/>
+      <c r="DV13" s="11"/>
+      <c r="DW13" s="11"/>
+      <c r="DX13" s="11"/>
+      <c r="DY13" s="11"/>
+      <c r="DZ13" s="11"/>
+      <c r="EA13" s="11"/>
+      <c r="EB13" s="11"/>
+      <c r="EC13" s="11"/>
+      <c r="ED13" s="11"/>
+      <c r="EE13" s="11"/>
+      <c r="EF13" s="11"/>
+      <c r="EG13" s="11"/>
+      <c r="EH13" s="11"/>
+      <c r="EI13" s="11"/>
+      <c r="EJ13" s="11"/>
+      <c r="EK13" s="11"/>
+      <c r="EL13" s="11"/>
+      <c r="EM13" s="11"/>
+      <c r="EN13" s="11"/>
+      <c r="EO13" s="11"/>
+      <c r="EP13" s="11"/>
+      <c r="EQ13" s="11"/>
+      <c r="ER13" s="11"/>
+      <c r="ES13" s="11"/>
+      <c r="ET13" s="11"/>
+      <c r="EU13" s="11"/>
+      <c r="EV13" s="11"/>
+      <c r="EW13" s="11"/>
+      <c r="EX13" s="11"/>
+      <c r="EY13" s="11"/>
+      <c r="EZ13" s="11"/>
+      <c r="FA13" s="11"/>
+      <c r="FB13" s="11"/>
+      <c r="FC13" s="11"/>
+      <c r="FD13" s="11"/>
+      <c r="FE13" s="11"/>
+      <c r="FF13" s="11"/>
+      <c r="FG13" s="11"/>
+      <c r="FH13" s="11"/>
+      <c r="FI13" s="11"/>
+      <c r="FJ13" s="11"/>
+      <c r="FK13" s="11"/>
+      <c r="FL13" s="11"/>
+      <c r="FM13" s="11"/>
+      <c r="FN13" s="11"/>
+      <c r="FO13" s="11"/>
+      <c r="FP13" s="11"/>
+      <c r="FQ13" s="11"/>
+      <c r="FR13" s="11"/>
+      <c r="FS13" s="11"/>
+      <c r="FT13" s="11"/>
+      <c r="FU13" s="11"/>
+      <c r="FV13" s="11"/>
+      <c r="FW13" s="11"/>
+      <c r="FX13" s="11"/>
+      <c r="FY13" s="11"/>
+      <c r="FZ13" s="11"/>
+      <c r="GA13" s="11"/>
+      <c r="GB13" s="11"/>
+      <c r="GC13" s="11"/>
+      <c r="GD13" s="11"/>
+      <c r="GE13" s="11"/>
+      <c r="GF13" s="11"/>
+      <c r="GG13" s="11"/>
+      <c r="GH13" s="11"/>
+      <c r="GI13" s="11"/>
+      <c r="GJ13" s="11"/>
+      <c r="GK13" s="11"/>
+      <c r="GL13" s="11"/>
+      <c r="GM13" s="11"/>
+      <c r="GN13" s="11"/>
+      <c r="GO13" s="11"/>
+      <c r="GP13" s="11"/>
+      <c r="GQ13" s="11"/>
+      <c r="GR13" s="11"/>
+      <c r="GS13" s="11"/>
+      <c r="GT13" s="11"/>
+      <c r="GU13" s="11"/>
+      <c r="GV13" s="11"/>
+      <c r="GW13" s="11"/>
+      <c r="GX13" s="11"/>
+      <c r="GY13" s="11"/>
+      <c r="GZ13" s="11"/>
+      <c r="HA13" s="11"/>
+      <c r="HB13" s="11"/>
+      <c r="HC13" s="11"/>
+      <c r="HD13" s="11"/>
+      <c r="HE13" s="11"/>
+      <c r="HF13" s="11"/>
+      <c r="HG13" s="11"/>
+      <c r="HH13" s="11"/>
+      <c r="HI13" s="11"/>
+      <c r="HJ13" s="11"/>
+      <c r="HK13" s="11"/>
+      <c r="HL13" s="11"/>
+      <c r="HM13" s="11"/>
+      <c r="HN13" s="11"/>
+      <c r="HO13" s="11"/>
+      <c r="HP13" s="11"/>
+      <c r="HQ13" s="11"/>
+      <c r="HR13" s="11"/>
+      <c r="HS13" s="11"/>
+      <c r="HT13" s="11"/>
+      <c r="HU13" s="11"/>
+      <c r="HV13" s="11"/>
+      <c r="HW13" s="11"/>
+      <c r="HX13" s="11"/>
+      <c r="HY13" s="11"/>
+      <c r="HZ13" s="11"/>
+      <c r="IA13" s="11"/>
+      <c r="IB13" s="11"/>
+      <c r="IC13" s="11"/>
+      <c r="ID13" s="11"/>
+      <c r="IE13" s="11"/>
+      <c r="IF13" s="11"/>
+      <c r="IG13" s="11"/>
+      <c r="IH13" s="11"/>
+      <c r="II13" s="11"/>
+      <c r="IJ13" s="11"/>
+      <c r="IK13" s="11"/>
+      <c r="IL13" s="11"/>
+      <c r="IM13" s="11"/>
+      <c r="IN13" s="11"/>
+      <c r="IO13" s="11"/>
+      <c r="IP13" s="11"/>
+      <c r="IQ13" s="11"/>
+      <c r="IR13" s="11"/>
+      <c r="IS13" s="11"/>
+      <c r="IT13" s="11"/>
+      <c r="IU13" s="11"/>
+      <c r="IV13" s="11"/>
     </row>
     <row r="14" spans="1:256" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -3999,306 +4716,553 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:256" s="17" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:256" s="12" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="16"/>
-      <c r="AE18" s="16"/>
-      <c r="AF18" s="16"/>
-      <c r="AG18" s="16"/>
-      <c r="AH18" s="16"/>
-      <c r="AI18" s="16"/>
-      <c r="AJ18" s="16"/>
-      <c r="AK18" s="16"/>
-      <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
-      <c r="AN18" s="16"/>
-      <c r="AO18" s="16"/>
-      <c r="AP18" s="16"/>
-      <c r="AQ18" s="16"/>
-      <c r="AR18" s="16"/>
-      <c r="AS18" s="16"/>
-      <c r="AT18" s="16"/>
-      <c r="AU18" s="16"/>
-      <c r="AV18" s="16"/>
-      <c r="AW18" s="16"/>
-      <c r="AX18" s="16"/>
-      <c r="AY18" s="16"/>
-      <c r="AZ18" s="16"/>
-      <c r="BA18" s="16"/>
-      <c r="BB18" s="16"/>
-      <c r="BC18" s="16"/>
-      <c r="BD18" s="16"/>
-      <c r="BE18" s="16"/>
-      <c r="BF18" s="16"/>
-      <c r="BG18" s="16"/>
-      <c r="BH18" s="16"/>
-      <c r="BI18" s="16"/>
-      <c r="BJ18" s="16"/>
-      <c r="BK18" s="16"/>
-      <c r="BL18" s="16"/>
-      <c r="BM18" s="16"/>
-      <c r="BN18" s="16"/>
-      <c r="BO18" s="16"/>
-      <c r="BP18" s="16"/>
-      <c r="BQ18" s="16"/>
-      <c r="BR18" s="16"/>
-      <c r="BS18" s="16"/>
-      <c r="BT18" s="16"/>
-      <c r="BU18" s="16"/>
-      <c r="BV18" s="16"/>
-      <c r="BW18" s="16"/>
-      <c r="BX18" s="16"/>
-      <c r="BY18" s="16"/>
-      <c r="BZ18" s="16"/>
-      <c r="CA18" s="16"/>
-      <c r="CB18" s="16"/>
-      <c r="CC18" s="16"/>
-      <c r="CD18" s="16"/>
-      <c r="CE18" s="16"/>
-      <c r="CF18" s="16"/>
-      <c r="CG18" s="16"/>
-      <c r="CH18" s="16"/>
-      <c r="CI18" s="16"/>
-      <c r="CJ18" s="16"/>
-      <c r="CK18" s="16"/>
-      <c r="CL18" s="16"/>
-      <c r="CM18" s="16"/>
-      <c r="CN18" s="16"/>
-      <c r="CO18" s="16"/>
-      <c r="CP18" s="16"/>
-      <c r="CQ18" s="16"/>
-      <c r="CR18" s="16"/>
-      <c r="CS18" s="16"/>
-      <c r="CT18" s="16"/>
-      <c r="CU18" s="16"/>
-      <c r="CV18" s="16"/>
-      <c r="CW18" s="16"/>
-      <c r="CX18" s="16"/>
-      <c r="CY18" s="16"/>
-      <c r="CZ18" s="16"/>
-      <c r="DA18" s="16"/>
-      <c r="DB18" s="16"/>
-      <c r="DC18" s="16"/>
-      <c r="DD18" s="16"/>
-      <c r="DE18" s="16"/>
-      <c r="DF18" s="16"/>
-      <c r="DG18" s="16"/>
-      <c r="DH18" s="16"/>
-      <c r="DI18" s="16"/>
-      <c r="DJ18" s="16"/>
-      <c r="DK18" s="16"/>
-      <c r="DL18" s="16"/>
-      <c r="DM18" s="16"/>
-      <c r="DN18" s="16"/>
-      <c r="DO18" s="16"/>
-      <c r="DP18" s="16"/>
-      <c r="DQ18" s="16"/>
-      <c r="DR18" s="16"/>
-      <c r="DS18" s="16"/>
-      <c r="DT18" s="16"/>
-      <c r="DU18" s="16"/>
-      <c r="DV18" s="16"/>
-      <c r="DW18" s="16"/>
-      <c r="DX18" s="16"/>
-      <c r="DY18" s="16"/>
-      <c r="DZ18" s="16"/>
-      <c r="EA18" s="16"/>
-      <c r="EB18" s="16"/>
-      <c r="EC18" s="16"/>
-      <c r="ED18" s="16"/>
-      <c r="EE18" s="16"/>
-      <c r="EF18" s="16"/>
-      <c r="EG18" s="16"/>
-      <c r="EH18" s="16"/>
-      <c r="EI18" s="16"/>
-      <c r="EJ18" s="16"/>
-      <c r="EK18" s="16"/>
-      <c r="EL18" s="16"/>
-      <c r="EM18" s="16"/>
-      <c r="EN18" s="16"/>
-      <c r="EO18" s="16"/>
-      <c r="EP18" s="16"/>
-      <c r="EQ18" s="16"/>
-      <c r="ER18" s="16"/>
-      <c r="ES18" s="16"/>
-      <c r="ET18" s="16"/>
-      <c r="EU18" s="16"/>
-      <c r="EV18" s="16"/>
-      <c r="EW18" s="16"/>
-      <c r="EX18" s="16"/>
-      <c r="EY18" s="16"/>
-      <c r="EZ18" s="16"/>
-      <c r="FA18" s="16"/>
-      <c r="FB18" s="16"/>
-      <c r="FC18" s="16"/>
-      <c r="FD18" s="16"/>
-      <c r="FE18" s="16"/>
-      <c r="FF18" s="16"/>
-      <c r="FG18" s="16"/>
-      <c r="FH18" s="16"/>
-      <c r="FI18" s="16"/>
-      <c r="FJ18" s="16"/>
-      <c r="FK18" s="16"/>
-      <c r="FL18" s="16"/>
-      <c r="FM18" s="16"/>
-      <c r="FN18" s="16"/>
-      <c r="FO18" s="16"/>
-      <c r="FP18" s="16"/>
-      <c r="FQ18" s="16"/>
-      <c r="FR18" s="16"/>
-      <c r="FS18" s="16"/>
-      <c r="FT18" s="16"/>
-      <c r="FU18" s="16"/>
-      <c r="FV18" s="16"/>
-      <c r="FW18" s="16"/>
-      <c r="FX18" s="16"/>
-      <c r="FY18" s="16"/>
-      <c r="FZ18" s="16"/>
-      <c r="GA18" s="16"/>
-      <c r="GB18" s="16"/>
-      <c r="GC18" s="16"/>
-      <c r="GD18" s="16"/>
-      <c r="GE18" s="16"/>
-      <c r="GF18" s="16"/>
-      <c r="GG18" s="16"/>
-      <c r="GH18" s="16"/>
-      <c r="GI18" s="16"/>
-      <c r="GJ18" s="16"/>
-      <c r="GK18" s="16"/>
-      <c r="GL18" s="16"/>
-      <c r="GM18" s="16"/>
-      <c r="GN18" s="16"/>
-      <c r="GO18" s="16"/>
-      <c r="GP18" s="16"/>
-      <c r="GQ18" s="16"/>
-      <c r="GR18" s="16"/>
-      <c r="GS18" s="16"/>
-      <c r="GT18" s="16"/>
-      <c r="GU18" s="16"/>
-      <c r="GV18" s="16"/>
-      <c r="GW18" s="16"/>
-      <c r="GX18" s="16"/>
-      <c r="GY18" s="16"/>
-      <c r="GZ18" s="16"/>
-      <c r="HA18" s="16"/>
-      <c r="HB18" s="16"/>
-      <c r="HC18" s="16"/>
-      <c r="HD18" s="16"/>
-      <c r="HE18" s="16"/>
-      <c r="HF18" s="16"/>
-      <c r="HG18" s="16"/>
-      <c r="HH18" s="16"/>
-      <c r="HI18" s="16"/>
-      <c r="HJ18" s="16"/>
-      <c r="HK18" s="16"/>
-      <c r="HL18" s="16"/>
-      <c r="HM18" s="16"/>
-      <c r="HN18" s="16"/>
-      <c r="HO18" s="16"/>
-      <c r="HP18" s="16"/>
-      <c r="HQ18" s="16"/>
-      <c r="HR18" s="16"/>
-      <c r="HS18" s="16"/>
-      <c r="HT18" s="16"/>
-      <c r="HU18" s="16"/>
-      <c r="HV18" s="16"/>
-      <c r="HW18" s="16"/>
-      <c r="HX18" s="16"/>
-      <c r="HY18" s="16"/>
-      <c r="HZ18" s="16"/>
-      <c r="IA18" s="16"/>
-      <c r="IB18" s="16"/>
-      <c r="IC18" s="16"/>
-      <c r="ID18" s="16"/>
-      <c r="IE18" s="16"/>
-      <c r="IF18" s="16"/>
-      <c r="IG18" s="16"/>
-      <c r="IH18" s="16"/>
-      <c r="II18" s="16"/>
-      <c r="IJ18" s="16"/>
-      <c r="IK18" s="16"/>
-      <c r="IL18" s="16"/>
-      <c r="IM18" s="16"/>
-      <c r="IN18" s="16"/>
-      <c r="IO18" s="16"/>
-      <c r="IP18" s="16"/>
-      <c r="IQ18" s="16"/>
-      <c r="IR18" s="16"/>
-      <c r="IS18" s="16"/>
-      <c r="IT18" s="16"/>
-      <c r="IU18" s="16"/>
-      <c r="IV18" s="16"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
+      <c r="AQ18" s="11"/>
+      <c r="AR18" s="11"/>
+      <c r="AS18" s="11"/>
+      <c r="AT18" s="11"/>
+      <c r="AU18" s="11"/>
+      <c r="AV18" s="11"/>
+      <c r="AW18" s="11"/>
+      <c r="AX18" s="11"/>
+      <c r="AY18" s="11"/>
+      <c r="AZ18" s="11"/>
+      <c r="BA18" s="11"/>
+      <c r="BB18" s="11"/>
+      <c r="BC18" s="11"/>
+      <c r="BD18" s="11"/>
+      <c r="BE18" s="11"/>
+      <c r="BF18" s="11"/>
+      <c r="BG18" s="11"/>
+      <c r="BH18" s="11"/>
+      <c r="BI18" s="11"/>
+      <c r="BJ18" s="11"/>
+      <c r="BK18" s="11"/>
+      <c r="BL18" s="11"/>
+      <c r="BM18" s="11"/>
+      <c r="BN18" s="11"/>
+      <c r="BO18" s="11"/>
+      <c r="BP18" s="11"/>
+      <c r="BQ18" s="11"/>
+      <c r="BR18" s="11"/>
+      <c r="BS18" s="11"/>
+      <c r="BT18" s="11"/>
+      <c r="BU18" s="11"/>
+      <c r="BV18" s="11"/>
+      <c r="BW18" s="11"/>
+      <c r="BX18" s="11"/>
+      <c r="BY18" s="11"/>
+      <c r="BZ18" s="11"/>
+      <c r="CA18" s="11"/>
+      <c r="CB18" s="11"/>
+      <c r="CC18" s="11"/>
+      <c r="CD18" s="11"/>
+      <c r="CE18" s="11"/>
+      <c r="CF18" s="11"/>
+      <c r="CG18" s="11"/>
+      <c r="CH18" s="11"/>
+      <c r="CI18" s="11"/>
+      <c r="CJ18" s="11"/>
+      <c r="CK18" s="11"/>
+      <c r="CL18" s="11"/>
+      <c r="CM18" s="11"/>
+      <c r="CN18" s="11"/>
+      <c r="CO18" s="11"/>
+      <c r="CP18" s="11"/>
+      <c r="CQ18" s="11"/>
+      <c r="CR18" s="11"/>
+      <c r="CS18" s="11"/>
+      <c r="CT18" s="11"/>
+      <c r="CU18" s="11"/>
+      <c r="CV18" s="11"/>
+      <c r="CW18" s="11"/>
+      <c r="CX18" s="11"/>
+      <c r="CY18" s="11"/>
+      <c r="CZ18" s="11"/>
+      <c r="DA18" s="11"/>
+      <c r="DB18" s="11"/>
+      <c r="DC18" s="11"/>
+      <c r="DD18" s="11"/>
+      <c r="DE18" s="11"/>
+      <c r="DF18" s="11"/>
+      <c r="DG18" s="11"/>
+      <c r="DH18" s="11"/>
+      <c r="DI18" s="11"/>
+      <c r="DJ18" s="11"/>
+      <c r="DK18" s="11"/>
+      <c r="DL18" s="11"/>
+      <c r="DM18" s="11"/>
+      <c r="DN18" s="11"/>
+      <c r="DO18" s="11"/>
+      <c r="DP18" s="11"/>
+      <c r="DQ18" s="11"/>
+      <c r="DR18" s="11"/>
+      <c r="DS18" s="11"/>
+      <c r="DT18" s="11"/>
+      <c r="DU18" s="11"/>
+      <c r="DV18" s="11"/>
+      <c r="DW18" s="11"/>
+      <c r="DX18" s="11"/>
+      <c r="DY18" s="11"/>
+      <c r="DZ18" s="11"/>
+      <c r="EA18" s="11"/>
+      <c r="EB18" s="11"/>
+      <c r="EC18" s="11"/>
+      <c r="ED18" s="11"/>
+      <c r="EE18" s="11"/>
+      <c r="EF18" s="11"/>
+      <c r="EG18" s="11"/>
+      <c r="EH18" s="11"/>
+      <c r="EI18" s="11"/>
+      <c r="EJ18" s="11"/>
+      <c r="EK18" s="11"/>
+      <c r="EL18" s="11"/>
+      <c r="EM18" s="11"/>
+      <c r="EN18" s="11"/>
+      <c r="EO18" s="11"/>
+      <c r="EP18" s="11"/>
+      <c r="EQ18" s="11"/>
+      <c r="ER18" s="11"/>
+      <c r="ES18" s="11"/>
+      <c r="ET18" s="11"/>
+      <c r="EU18" s="11"/>
+      <c r="EV18" s="11"/>
+      <c r="EW18" s="11"/>
+      <c r="EX18" s="11"/>
+      <c r="EY18" s="11"/>
+      <c r="EZ18" s="11"/>
+      <c r="FA18" s="11"/>
+      <c r="FB18" s="11"/>
+      <c r="FC18" s="11"/>
+      <c r="FD18" s="11"/>
+      <c r="FE18" s="11"/>
+      <c r="FF18" s="11"/>
+      <c r="FG18" s="11"/>
+      <c r="FH18" s="11"/>
+      <c r="FI18" s="11"/>
+      <c r="FJ18" s="11"/>
+      <c r="FK18" s="11"/>
+      <c r="FL18" s="11"/>
+      <c r="FM18" s="11"/>
+      <c r="FN18" s="11"/>
+      <c r="FO18" s="11"/>
+      <c r="FP18" s="11"/>
+      <c r="FQ18" s="11"/>
+      <c r="FR18" s="11"/>
+      <c r="FS18" s="11"/>
+      <c r="FT18" s="11"/>
+      <c r="FU18" s="11"/>
+      <c r="FV18" s="11"/>
+      <c r="FW18" s="11"/>
+      <c r="FX18" s="11"/>
+      <c r="FY18" s="11"/>
+      <c r="FZ18" s="11"/>
+      <c r="GA18" s="11"/>
+      <c r="GB18" s="11"/>
+      <c r="GC18" s="11"/>
+      <c r="GD18" s="11"/>
+      <c r="GE18" s="11"/>
+      <c r="GF18" s="11"/>
+      <c r="GG18" s="11"/>
+      <c r="GH18" s="11"/>
+      <c r="GI18" s="11"/>
+      <c r="GJ18" s="11"/>
+      <c r="GK18" s="11"/>
+      <c r="GL18" s="11"/>
+      <c r="GM18" s="11"/>
+      <c r="GN18" s="11"/>
+      <c r="GO18" s="11"/>
+      <c r="GP18" s="11"/>
+      <c r="GQ18" s="11"/>
+      <c r="GR18" s="11"/>
+      <c r="GS18" s="11"/>
+      <c r="GT18" s="11"/>
+      <c r="GU18" s="11"/>
+      <c r="GV18" s="11"/>
+      <c r="GW18" s="11"/>
+      <c r="GX18" s="11"/>
+      <c r="GY18" s="11"/>
+      <c r="GZ18" s="11"/>
+      <c r="HA18" s="11"/>
+      <c r="HB18" s="11"/>
+      <c r="HC18" s="11"/>
+      <c r="HD18" s="11"/>
+      <c r="HE18" s="11"/>
+      <c r="HF18" s="11"/>
+      <c r="HG18" s="11"/>
+      <c r="HH18" s="11"/>
+      <c r="HI18" s="11"/>
+      <c r="HJ18" s="11"/>
+      <c r="HK18" s="11"/>
+      <c r="HL18" s="11"/>
+      <c r="HM18" s="11"/>
+      <c r="HN18" s="11"/>
+      <c r="HO18" s="11"/>
+      <c r="HP18" s="11"/>
+      <c r="HQ18" s="11"/>
+      <c r="HR18" s="11"/>
+      <c r="HS18" s="11"/>
+      <c r="HT18" s="11"/>
+      <c r="HU18" s="11"/>
+      <c r="HV18" s="11"/>
+      <c r="HW18" s="11"/>
+      <c r="HX18" s="11"/>
+      <c r="HY18" s="11"/>
+      <c r="HZ18" s="11"/>
+      <c r="IA18" s="11"/>
+      <c r="IB18" s="11"/>
+      <c r="IC18" s="11"/>
+      <c r="ID18" s="11"/>
+      <c r="IE18" s="11"/>
+      <c r="IF18" s="11"/>
+      <c r="IG18" s="11"/>
+      <c r="IH18" s="11"/>
+      <c r="II18" s="11"/>
+      <c r="IJ18" s="11"/>
+      <c r="IK18" s="11"/>
+      <c r="IL18" s="11"/>
+      <c r="IM18" s="11"/>
+      <c r="IN18" s="11"/>
+      <c r="IO18" s="11"/>
+      <c r="IP18" s="11"/>
+      <c r="IQ18" s="11"/>
+      <c r="IR18" s="11"/>
+      <c r="IS18" s="11"/>
+      <c r="IT18" s="11"/>
+      <c r="IU18" s="11"/>
+      <c r="IV18" s="11"/>
     </row>
-    <row r="19" spans="1:256" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:256" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="11"/>
+      <c r="AR19" s="11"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="11"/>
+      <c r="AV19" s="11"/>
+      <c r="AW19" s="11"/>
+      <c r="AX19" s="11"/>
+      <c r="AY19" s="11"/>
+      <c r="AZ19" s="11"/>
+      <c r="BA19" s="11"/>
+      <c r="BB19" s="11"/>
+      <c r="BC19" s="11"/>
+      <c r="BD19" s="11"/>
+      <c r="BE19" s="11"/>
+      <c r="BF19" s="11"/>
+      <c r="BG19" s="11"/>
+      <c r="BH19" s="11"/>
+      <c r="BI19" s="11"/>
+      <c r="BJ19" s="11"/>
+      <c r="BK19" s="11"/>
+      <c r="BL19" s="11"/>
+      <c r="BM19" s="11"/>
+      <c r="BN19" s="11"/>
+      <c r="BO19" s="11"/>
+      <c r="BP19" s="11"/>
+      <c r="BQ19" s="11"/>
+      <c r="BR19" s="11"/>
+      <c r="BS19" s="11"/>
+      <c r="BT19" s="11"/>
+      <c r="BU19" s="11"/>
+      <c r="BV19" s="11"/>
+      <c r="BW19" s="11"/>
+      <c r="BX19" s="11"/>
+      <c r="BY19" s="11"/>
+      <c r="BZ19" s="11"/>
+      <c r="CA19" s="11"/>
+      <c r="CB19" s="11"/>
+      <c r="CC19" s="11"/>
+      <c r="CD19" s="11"/>
+      <c r="CE19" s="11"/>
+      <c r="CF19" s="11"/>
+      <c r="CG19" s="11"/>
+      <c r="CH19" s="11"/>
+      <c r="CI19" s="11"/>
+      <c r="CJ19" s="11"/>
+      <c r="CK19" s="11"/>
+      <c r="CL19" s="11"/>
+      <c r="CM19" s="11"/>
+      <c r="CN19" s="11"/>
+      <c r="CO19" s="11"/>
+      <c r="CP19" s="11"/>
+      <c r="CQ19" s="11"/>
+      <c r="CR19" s="11"/>
+      <c r="CS19" s="11"/>
+      <c r="CT19" s="11"/>
+      <c r="CU19" s="11"/>
+      <c r="CV19" s="11"/>
+      <c r="CW19" s="11"/>
+      <c r="CX19" s="11"/>
+      <c r="CY19" s="11"/>
+      <c r="CZ19" s="11"/>
+      <c r="DA19" s="11"/>
+      <c r="DB19" s="11"/>
+      <c r="DC19" s="11"/>
+      <c r="DD19" s="11"/>
+      <c r="DE19" s="11"/>
+      <c r="DF19" s="11"/>
+      <c r="DG19" s="11"/>
+      <c r="DH19" s="11"/>
+      <c r="DI19" s="11"/>
+      <c r="DJ19" s="11"/>
+      <c r="DK19" s="11"/>
+      <c r="DL19" s="11"/>
+      <c r="DM19" s="11"/>
+      <c r="DN19" s="11"/>
+      <c r="DO19" s="11"/>
+      <c r="DP19" s="11"/>
+      <c r="DQ19" s="11"/>
+      <c r="DR19" s="11"/>
+      <c r="DS19" s="11"/>
+      <c r="DT19" s="11"/>
+      <c r="DU19" s="11"/>
+      <c r="DV19" s="11"/>
+      <c r="DW19" s="11"/>
+      <c r="DX19" s="11"/>
+      <c r="DY19" s="11"/>
+      <c r="DZ19" s="11"/>
+      <c r="EA19" s="11"/>
+      <c r="EB19" s="11"/>
+      <c r="EC19" s="11"/>
+      <c r="ED19" s="11"/>
+      <c r="EE19" s="11"/>
+      <c r="EF19" s="11"/>
+      <c r="EG19" s="11"/>
+      <c r="EH19" s="11"/>
+      <c r="EI19" s="11"/>
+      <c r="EJ19" s="11"/>
+      <c r="EK19" s="11"/>
+      <c r="EL19" s="11"/>
+      <c r="EM19" s="11"/>
+      <c r="EN19" s="11"/>
+      <c r="EO19" s="11"/>
+      <c r="EP19" s="11"/>
+      <c r="EQ19" s="11"/>
+      <c r="ER19" s="11"/>
+      <c r="ES19" s="11"/>
+      <c r="ET19" s="11"/>
+      <c r="EU19" s="11"/>
+      <c r="EV19" s="11"/>
+      <c r="EW19" s="11"/>
+      <c r="EX19" s="11"/>
+      <c r="EY19" s="11"/>
+      <c r="EZ19" s="11"/>
+      <c r="FA19" s="11"/>
+      <c r="FB19" s="11"/>
+      <c r="FC19" s="11"/>
+      <c r="FD19" s="11"/>
+      <c r="FE19" s="11"/>
+      <c r="FF19" s="11"/>
+      <c r="FG19" s="11"/>
+      <c r="FH19" s="11"/>
+      <c r="FI19" s="11"/>
+      <c r="FJ19" s="11"/>
+      <c r="FK19" s="11"/>
+      <c r="FL19" s="11"/>
+      <c r="FM19" s="11"/>
+      <c r="FN19" s="11"/>
+      <c r="FO19" s="11"/>
+      <c r="FP19" s="11"/>
+      <c r="FQ19" s="11"/>
+      <c r="FR19" s="11"/>
+      <c r="FS19" s="11"/>
+      <c r="FT19" s="11"/>
+      <c r="FU19" s="11"/>
+      <c r="FV19" s="11"/>
+      <c r="FW19" s="11"/>
+      <c r="FX19" s="11"/>
+      <c r="FY19" s="11"/>
+      <c r="FZ19" s="11"/>
+      <c r="GA19" s="11"/>
+      <c r="GB19" s="11"/>
+      <c r="GC19" s="11"/>
+      <c r="GD19" s="11"/>
+      <c r="GE19" s="11"/>
+      <c r="GF19" s="11"/>
+      <c r="GG19" s="11"/>
+      <c r="GH19" s="11"/>
+      <c r="GI19" s="11"/>
+      <c r="GJ19" s="11"/>
+      <c r="GK19" s="11"/>
+      <c r="GL19" s="11"/>
+      <c r="GM19" s="11"/>
+      <c r="GN19" s="11"/>
+      <c r="GO19" s="11"/>
+      <c r="GP19" s="11"/>
+      <c r="GQ19" s="11"/>
+      <c r="GR19" s="11"/>
+      <c r="GS19" s="11"/>
+      <c r="GT19" s="11"/>
+      <c r="GU19" s="11"/>
+      <c r="GV19" s="11"/>
+      <c r="GW19" s="11"/>
+      <c r="GX19" s="11"/>
+      <c r="GY19" s="11"/>
+      <c r="GZ19" s="11"/>
+      <c r="HA19" s="11"/>
+      <c r="HB19" s="11"/>
+      <c r="HC19" s="11"/>
+      <c r="HD19" s="11"/>
+      <c r="HE19" s="11"/>
+      <c r="HF19" s="11"/>
+      <c r="HG19" s="11"/>
+      <c r="HH19" s="11"/>
+      <c r="HI19" s="11"/>
+      <c r="HJ19" s="11"/>
+      <c r="HK19" s="11"/>
+      <c r="HL19" s="11"/>
+      <c r="HM19" s="11"/>
+      <c r="HN19" s="11"/>
+      <c r="HO19" s="11"/>
+      <c r="HP19" s="11"/>
+      <c r="HQ19" s="11"/>
+      <c r="HR19" s="11"/>
+      <c r="HS19" s="11"/>
+      <c r="HT19" s="11"/>
+      <c r="HU19" s="11"/>
+      <c r="HV19" s="11"/>
+      <c r="HW19" s="11"/>
+      <c r="HX19" s="11"/>
+      <c r="HY19" s="11"/>
+      <c r="HZ19" s="11"/>
+      <c r="IA19" s="11"/>
+      <c r="IB19" s="11"/>
+      <c r="IC19" s="11"/>
+      <c r="ID19" s="11"/>
+      <c r="IE19" s="11"/>
+      <c r="IF19" s="11"/>
+      <c r="IG19" s="11"/>
+      <c r="IH19" s="11"/>
+      <c r="II19" s="11"/>
+      <c r="IJ19" s="11"/>
+      <c r="IK19" s="11"/>
+      <c r="IL19" s="11"/>
+      <c r="IM19" s="11"/>
+      <c r="IN19" s="11"/>
+      <c r="IO19" s="11"/>
+      <c r="IP19" s="11"/>
+      <c r="IQ19" s="11"/>
+      <c r="IR19" s="11"/>
+      <c r="IS19" s="11"/>
+      <c r="IT19" s="11"/>
+      <c r="IU19" s="11"/>
+      <c r="IV19" s="11"/>
     </row>
     <row r="20" spans="1:256" s="12" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -4576,28 +5540,275 @@
       <c r="IU20" s="11"/>
       <c r="IV20" s="11"/>
     </row>
-    <row r="21" spans="1:256" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:256" s="12" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="11"/>
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="11"/>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="11"/>
+      <c r="AR21" s="11"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="11"/>
+      <c r="AU21" s="11"/>
+      <c r="AV21" s="11"/>
+      <c r="AW21" s="11"/>
+      <c r="AX21" s="11"/>
+      <c r="AY21" s="11"/>
+      <c r="AZ21" s="11"/>
+      <c r="BA21" s="11"/>
+      <c r="BB21" s="11"/>
+      <c r="BC21" s="11"/>
+      <c r="BD21" s="11"/>
+      <c r="BE21" s="11"/>
+      <c r="BF21" s="11"/>
+      <c r="BG21" s="11"/>
+      <c r="BH21" s="11"/>
+      <c r="BI21" s="11"/>
+      <c r="BJ21" s="11"/>
+      <c r="BK21" s="11"/>
+      <c r="BL21" s="11"/>
+      <c r="BM21" s="11"/>
+      <c r="BN21" s="11"/>
+      <c r="BO21" s="11"/>
+      <c r="BP21" s="11"/>
+      <c r="BQ21" s="11"/>
+      <c r="BR21" s="11"/>
+      <c r="BS21" s="11"/>
+      <c r="BT21" s="11"/>
+      <c r="BU21" s="11"/>
+      <c r="BV21" s="11"/>
+      <c r="BW21" s="11"/>
+      <c r="BX21" s="11"/>
+      <c r="BY21" s="11"/>
+      <c r="BZ21" s="11"/>
+      <c r="CA21" s="11"/>
+      <c r="CB21" s="11"/>
+      <c r="CC21" s="11"/>
+      <c r="CD21" s="11"/>
+      <c r="CE21" s="11"/>
+      <c r="CF21" s="11"/>
+      <c r="CG21" s="11"/>
+      <c r="CH21" s="11"/>
+      <c r="CI21" s="11"/>
+      <c r="CJ21" s="11"/>
+      <c r="CK21" s="11"/>
+      <c r="CL21" s="11"/>
+      <c r="CM21" s="11"/>
+      <c r="CN21" s="11"/>
+      <c r="CO21" s="11"/>
+      <c r="CP21" s="11"/>
+      <c r="CQ21" s="11"/>
+      <c r="CR21" s="11"/>
+      <c r="CS21" s="11"/>
+      <c r="CT21" s="11"/>
+      <c r="CU21" s="11"/>
+      <c r="CV21" s="11"/>
+      <c r="CW21" s="11"/>
+      <c r="CX21" s="11"/>
+      <c r="CY21" s="11"/>
+      <c r="CZ21" s="11"/>
+      <c r="DA21" s="11"/>
+      <c r="DB21" s="11"/>
+      <c r="DC21" s="11"/>
+      <c r="DD21" s="11"/>
+      <c r="DE21" s="11"/>
+      <c r="DF21" s="11"/>
+      <c r="DG21" s="11"/>
+      <c r="DH21" s="11"/>
+      <c r="DI21" s="11"/>
+      <c r="DJ21" s="11"/>
+      <c r="DK21" s="11"/>
+      <c r="DL21" s="11"/>
+      <c r="DM21" s="11"/>
+      <c r="DN21" s="11"/>
+      <c r="DO21" s="11"/>
+      <c r="DP21" s="11"/>
+      <c r="DQ21" s="11"/>
+      <c r="DR21" s="11"/>
+      <c r="DS21" s="11"/>
+      <c r="DT21" s="11"/>
+      <c r="DU21" s="11"/>
+      <c r="DV21" s="11"/>
+      <c r="DW21" s="11"/>
+      <c r="DX21" s="11"/>
+      <c r="DY21" s="11"/>
+      <c r="DZ21" s="11"/>
+      <c r="EA21" s="11"/>
+      <c r="EB21" s="11"/>
+      <c r="EC21" s="11"/>
+      <c r="ED21" s="11"/>
+      <c r="EE21" s="11"/>
+      <c r="EF21" s="11"/>
+      <c r="EG21" s="11"/>
+      <c r="EH21" s="11"/>
+      <c r="EI21" s="11"/>
+      <c r="EJ21" s="11"/>
+      <c r="EK21" s="11"/>
+      <c r="EL21" s="11"/>
+      <c r="EM21" s="11"/>
+      <c r="EN21" s="11"/>
+      <c r="EO21" s="11"/>
+      <c r="EP21" s="11"/>
+      <c r="EQ21" s="11"/>
+      <c r="ER21" s="11"/>
+      <c r="ES21" s="11"/>
+      <c r="ET21" s="11"/>
+      <c r="EU21" s="11"/>
+      <c r="EV21" s="11"/>
+      <c r="EW21" s="11"/>
+      <c r="EX21" s="11"/>
+      <c r="EY21" s="11"/>
+      <c r="EZ21" s="11"/>
+      <c r="FA21" s="11"/>
+      <c r="FB21" s="11"/>
+      <c r="FC21" s="11"/>
+      <c r="FD21" s="11"/>
+      <c r="FE21" s="11"/>
+      <c r="FF21" s="11"/>
+      <c r="FG21" s="11"/>
+      <c r="FH21" s="11"/>
+      <c r="FI21" s="11"/>
+      <c r="FJ21" s="11"/>
+      <c r="FK21" s="11"/>
+      <c r="FL21" s="11"/>
+      <c r="FM21" s="11"/>
+      <c r="FN21" s="11"/>
+      <c r="FO21" s="11"/>
+      <c r="FP21" s="11"/>
+      <c r="FQ21" s="11"/>
+      <c r="FR21" s="11"/>
+      <c r="FS21" s="11"/>
+      <c r="FT21" s="11"/>
+      <c r="FU21" s="11"/>
+      <c r="FV21" s="11"/>
+      <c r="FW21" s="11"/>
+      <c r="FX21" s="11"/>
+      <c r="FY21" s="11"/>
+      <c r="FZ21" s="11"/>
+      <c r="GA21" s="11"/>
+      <c r="GB21" s="11"/>
+      <c r="GC21" s="11"/>
+      <c r="GD21" s="11"/>
+      <c r="GE21" s="11"/>
+      <c r="GF21" s="11"/>
+      <c r="GG21" s="11"/>
+      <c r="GH21" s="11"/>
+      <c r="GI21" s="11"/>
+      <c r="GJ21" s="11"/>
+      <c r="GK21" s="11"/>
+      <c r="GL21" s="11"/>
+      <c r="GM21" s="11"/>
+      <c r="GN21" s="11"/>
+      <c r="GO21" s="11"/>
+      <c r="GP21" s="11"/>
+      <c r="GQ21" s="11"/>
+      <c r="GR21" s="11"/>
+      <c r="GS21" s="11"/>
+      <c r="GT21" s="11"/>
+      <c r="GU21" s="11"/>
+      <c r="GV21" s="11"/>
+      <c r="GW21" s="11"/>
+      <c r="GX21" s="11"/>
+      <c r="GY21" s="11"/>
+      <c r="GZ21" s="11"/>
+      <c r="HA21" s="11"/>
+      <c r="HB21" s="11"/>
+      <c r="HC21" s="11"/>
+      <c r="HD21" s="11"/>
+      <c r="HE21" s="11"/>
+      <c r="HF21" s="11"/>
+      <c r="HG21" s="11"/>
+      <c r="HH21" s="11"/>
+      <c r="HI21" s="11"/>
+      <c r="HJ21" s="11"/>
+      <c r="HK21" s="11"/>
+      <c r="HL21" s="11"/>
+      <c r="HM21" s="11"/>
+      <c r="HN21" s="11"/>
+      <c r="HO21" s="11"/>
+      <c r="HP21" s="11"/>
+      <c r="HQ21" s="11"/>
+      <c r="HR21" s="11"/>
+      <c r="HS21" s="11"/>
+      <c r="HT21" s="11"/>
+      <c r="HU21" s="11"/>
+      <c r="HV21" s="11"/>
+      <c r="HW21" s="11"/>
+      <c r="HX21" s="11"/>
+      <c r="HY21" s="11"/>
+      <c r="HZ21" s="11"/>
+      <c r="IA21" s="11"/>
+      <c r="IB21" s="11"/>
+      <c r="IC21" s="11"/>
+      <c r="ID21" s="11"/>
+      <c r="IE21" s="11"/>
+      <c r="IF21" s="11"/>
+      <c r="IG21" s="11"/>
+      <c r="IH21" s="11"/>
+      <c r="II21" s="11"/>
+      <c r="IJ21" s="11"/>
+      <c r="IK21" s="11"/>
+      <c r="IL21" s="11"/>
+      <c r="IM21" s="11"/>
+      <c r="IN21" s="11"/>
+      <c r="IO21" s="11"/>
+      <c r="IP21" s="11"/>
+      <c r="IQ21" s="11"/>
+      <c r="IR21" s="11"/>
+      <c r="IS21" s="11"/>
+      <c r="IT21" s="11"/>
+      <c r="IU21" s="11"/>
+      <c r="IV21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>